<commit_message>
Excel Read From File
</commit_message>
<xml_diff>
--- a/cplex/PeriodicModel2/multi-period-resourceV2.xlsx
+++ b/cplex/PeriodicModel2/multi-period-resourceV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catmailohio-my.sharepoint.com/personal/sormaz_ohio_edu/Documents/sormaz/Graduate-students/ise-ms-sormaz-advisor/malik/malik-shared/PhD - Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\hospital-simulation\cplex\PeriodicModel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="890" documentId="8_{8ADDBD1B-25AC-40FB-B67D-474459341872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A222BF1-803D-48EE-89AE-CB4CB81830B5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F195AA2-72D7-4A48-8EB2-6AE7DAEDEB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D7907A3-E876-4FA6-B9C6-209E690F9D0D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{2D7907A3-E876-4FA6-B9C6-209E690F9D0D}"/>
   </bookViews>
   <sheets>
     <sheet name="dp-method (2)" sheetId="5" r:id="rId1"/>
@@ -19,118 +19,119 @@
     <sheet name="dp-method" sheetId="3" r:id="rId4"/>
     <sheet name="IP-Method-C3 (2)" sheetId="4" r:id="rId5"/>
     <sheet name="Answer Report 1" sheetId="2" r:id="rId6"/>
-    <sheet name="IP-Method-C3" sheetId="1" r:id="rId7"/>
-    <sheet name="dp-method-dns" sheetId="8" r:id="rId8"/>
+    <sheet name="Data" sheetId="1" r:id="rId7"/>
+    <sheet name="Type" sheetId="10" r:id="rId8"/>
+    <sheet name="dp-method-dns" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">Data!$M$3:$M$22</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'dp-method'!$M$3:$M$6</definedName>
-    <definedName name="solver_adj" localSheetId="6" hidden="1">'IP-Method-C3'!$M$3:$M$22</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$M$3:$M$22</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">Data!$B$24:$K$26</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'dp-method'!$M$18</definedName>
-    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'IP-Method-C3'!$B$24:$K$26</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$B$24:$K$24</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">Data!$M$3:$M$22</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'dp-method'!$M$3:$M$7</definedName>
-    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'IP-Method-C3'!$M$3:$M$22</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$M$3:$M$22</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$M$3:$M$22</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">Data!$M$26</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'dp-method'!$L$18</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'dp-method (2)'!$E$3</definedName>
-    <definedName name="solver_opt" localSheetId="6" hidden="1">'IP-Method-C3'!$M$26</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$M$26</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">'dp-method'!$C$12</definedName>
-    <definedName name="solver_rhs1" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">'IP-Method-C3 (2)'!$B$26</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="210">
   <si>
     <t>patient</t>
   </si>
@@ -810,6 +811,12 @@
   </si>
   <si>
     <t>AHLP</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Patient</t>
   </si>
 </sst>
 </file>
@@ -982,10 +989,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1287,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF1C81-1E65-438D-A200-356ECF7698DE}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
@@ -2160,7 +2163,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4920,7 +4923,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5510,6 +5513,166 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926A9B14-2741-42FB-8964-8009030A07D5}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E475F4-6695-48AF-BC69-EC078A440803}">
   <dimension ref="A1:I45"/>
   <sheetViews>

</xml_diff>